<commit_message>
Droped EPPlus for NPOI
</commit_message>
<xml_diff>
--- a/Sample Data/Test.xlsx
+++ b/Sample Data/Test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40016" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40018" uniqueCount="114">
   <si>
     <t>#</t>
   </si>
@@ -339,31 +339,27 @@
   </si>
   <si>
     <t>Alkire</t>
+  </si>
+  <si>
+    <t>Minor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblData" displayName="tblData" ref="A1:H5001" totalsRowShown="0">
-  <autoFilter ref="A1:H5001">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblData" displayName="tblData" ref="E6:M5006" totalsRowShown="0">
+  <tableColumns count="9">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="First Name"/>
     <tableColumn id="3" name="Last Name"/>
     <tableColumn id="4" name="Gender"/>
     <tableColumn id="5" name="Country"/>
     <tableColumn id="6" name="Age"/>
-    <tableColumn id="7" name="Date" dataDxfId="0"/>
+    <tableColumn id="7" name="Date" dataDxfId="1"/>
     <tableColumn id="8" name="Id"/>
+    <tableColumn id="9" name="Minor" dataDxfId="0">
+      <calculatedColumnFormula>tblData[[#This Row],[Age]]&lt;18</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>

</xml_diff>